<commit_message>
Updated version to 1.0
</commit_message>
<xml_diff>
--- a/替换词表.xlsx
+++ b/替换词表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\KnoLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4663163D-1A3A-455E-A2AD-B57151526731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8D787F-9296-40C1-A88F-0E72C7413C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,10 +89,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否为主持人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cici</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,6 +111,10 @@
       </rPr>
       <t>**Cici**</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否为昵称列</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -515,10 +515,10 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>

</xml_diff>